<commit_message>
update to technoeconomics tables
</commit_message>
<xml_diff>
--- a/model_considerations/Technoeconomics overview.xlsx
+++ b/model_considerations/Technoeconomics overview.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s203679_dtu_dk/Documents/Dokumenter/DTU_Man/h2_system_dynamics/model_considerations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="373" documentId="8_{B4D2D1A9-8B8E-4336-848C-F25BE913BA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C32B852-D9C6-4C44-8E6C-DA3BBF98E373}"/>
+  <xr:revisionPtr revIDLastSave="473" documentId="8_{B4D2D1A9-8B8E-4336-848C-F25BE913BA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4CC9344-17D2-4552-A734-DCE8C69487A2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{1D0F97FC-33C4-4FEB-A6BA-2EB9839B62D8}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{1D0F97FC-33C4-4FEB-A6BA-2EB9839B62D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sector Activity Assumptions" sheetId="2" r:id="rId1"/>
     <sheet name="Levelized Production Costs" sheetId="1" r:id="rId2"/>
     <sheet name="Transport Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="Fuel Costs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="188">
   <si>
     <t>Technology</t>
   </si>
@@ -452,6 +453,156 @@
   </si>
   <si>
     <t xml:space="preserve"> https://www.petrochemistry.eu/about-petrochemistry/petrochemicals-facts-and-figures/european-market-overview/.</t>
+  </si>
+  <si>
+    <t>https://www.clean-hydrogen.europa.eu/media/publications/study-hydrogen-ports-and-industrial-coastal-areas-reports_en</t>
+  </si>
+  <si>
+    <t>eurostat</t>
+  </si>
+  <si>
+    <t>Transport Sector</t>
+  </si>
+  <si>
+    <t>Cost metric</t>
+  </si>
+  <si>
+    <t>Fuel cost</t>
+  </si>
+  <si>
+    <t>€/km</t>
+  </si>
+  <si>
+    <t>M€/yr</t>
+  </si>
+  <si>
+    <t>SEAMAPS</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.apenergy.2021.118079</t>
+  </si>
+  <si>
+    <t>Renewable Kerosene</t>
+  </si>
+  <si>
+    <t>Jetfuel €/GJ</t>
+  </si>
+  <si>
+    <t>CO2 Price</t>
+  </si>
+  <si>
+    <t>Electricity Price</t>
+  </si>
+  <si>
+    <t>Carbon Tax</t>
+  </si>
+  <si>
+    <t>Coal Price</t>
+  </si>
+  <si>
+    <t>Gas Price</t>
+  </si>
+  <si>
+    <t>Biomass Price</t>
+  </si>
+  <si>
+    <t>Biooil Price</t>
+  </si>
+  <si>
+    <t>Grid Electricity Emissions</t>
+  </si>
+  <si>
+    <t>Jetfuel Price</t>
+  </si>
+  <si>
+    <t>Naphtha Price</t>
+  </si>
+  <si>
+    <t>HFO Price</t>
+  </si>
+  <si>
+    <t>Diesel Price</t>
+  </si>
+  <si>
+    <t>Data Input</t>
+  </si>
+  <si>
+    <t>PS Capture Cost</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>40 €/MWh</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t>\cite{heatmap_eu}</t>
+  </si>
+  <si>
+    <t>\cite{EAAnalyses2013}</t>
+  </si>
+  <si>
+    <t>Austrian Chamber of Agriculture. 2023. Lower Austria wood market week 09/2023. Available at: 〈https://www.lko.at/holz+2400++1298002〉</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S2212982023001749?ref=pdf_download&amp;fr=RR-2&amp;rr=914784664b2cbe47#bib37</t>
+  </si>
+  <si>
+    <t>Projections from EA in 2013 still seem somewhat in line with current prices. Keep assumption.</t>
+  </si>
+  <si>
+    <t>Source for historical cost: (around 900 $/t (25 $/GJ assuming LHV of 36 GJ/t) in 2024)</t>
+  </si>
+  <si>
+    <t>https://www.spglobal.com/commodityinsights/en/market-insights/latest-news/agriculture/100423-global-uco-supply-to-double-by-2030-as-us-eu-policies-drive-asian-supply</t>
+  </si>
+  <si>
+    <t>20 €/MWh</t>
+  </si>
+  <si>
+    <t>Waste Heat Value</t>
+  </si>
+  <si>
+    <t>IEA WEO NZE</t>
+  </si>
+  <si>
+    <t>60-204 €/tCO2</t>
+  </si>
+  <si>
+    <t>https://ens.dk/en/our-services/statistics-data-key-figures-and-energy-maps/key-figures</t>
+  </si>
+  <si>
+    <t>Maybe get values from Balmorel</t>
+  </si>
+  <si>
+    <t>0.2 tCO2/MWh</t>
+  </si>
+  <si>
+    <t>Oil+30% crack spread</t>
+  </si>
+  <si>
+    <t>\cite{iata_fuel_fact_sheet}</t>
+  </si>
+  <si>
+    <t>\cite{trading_economics_naphtha}</t>
+  </si>
+  <si>
+    <t>Equal to crude oil price</t>
+  </si>
+  <si>
+    <t>1.2 €/l</t>
+  </si>
+  <si>
+    <t>Follows Crude Oil prices otherwise</t>
+  </si>
+  <si>
+    <t>Oil+10% crack spread</t>
+  </si>
+  <si>
+    <t>Crude Oil Price</t>
   </si>
 </sst>
 </file>
@@ -655,7 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -693,7 +844,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -713,6 +863,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1054,18 +1206,18 @@
   <dimension ref="B2:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C2" sqref="C2:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="147.453125" customWidth="1"/>
+    <col min="6" max="6" width="147.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1082,16 +1234,16 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="32"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1108,7 +1260,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1125,7 +1277,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
@@ -1138,11 +1290,11 @@
       <c r="E6" s="5">
         <v>19.100000000000001</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="40" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
@@ -1155,11 +1307,11 @@
       <c r="E7" s="5">
         <v>96</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="37" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
@@ -1176,7 +1328,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
@@ -1189,18 +1341,20 @@
       <c r="E9" s="5">
         <v>2.9</v>
       </c>
-      <c r="F9" s="29"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F9" s="40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="32"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F10" s="31"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
@@ -1213,9 +1367,11 @@
       <c r="E11" s="5">
         <v>928</v>
       </c>
-      <c r="F11" s="29"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F11" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
@@ -1228,9 +1384,11 @@
       <c r="E12" s="5">
         <v>131</v>
       </c>
-      <c r="F12" s="29"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F12" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
@@ -1243,9 +1401,11 @@
       <c r="E13" s="5">
         <v>4380</v>
       </c>
-      <c r="F13" s="29"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F13" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>21</v>
       </c>
@@ -1258,9 +1418,11 @@
       <c r="E14" s="5">
         <v>1620</v>
       </c>
-      <c r="F14" s="29"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F14" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>18</v>
       </c>
@@ -1273,9 +1435,11 @@
       <c r="E15" s="5">
         <v>664</v>
       </c>
-      <c r="F15" s="29"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F15" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
@@ -1288,9 +1452,15 @@
       <c r="E16" s="6">
         <v>96</v>
       </c>
-      <c r="F16" s="31"/>
+      <c r="F16" s="29" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{61CFE02B-0F47-4013-BAC8-D68E3E9D357B}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{95355CDB-7C9E-4AAF-A789-4253DC190C17}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1299,66 +1469,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38DB609-11F6-4767-9B6F-02B754BF68D0}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="43.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.7265625" customWidth="1"/>
-    <col min="13" max="13" width="96.7265625" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.7109375" customWidth="1"/>
+    <col min="13" max="13" width="96.7109375" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="39"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="39"/>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
       <c r="B2" s="22"/>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
-      <c r="N2" s="39"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="39"/>
+      <c r="N2" s="38"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
       <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
@@ -1395,16 +1565,16 @@
       <c r="M3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="N3" s="39" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="39"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
       <c r="B4" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>55</v>
       </c>
       <c r="D4" t="s">
@@ -1431,22 +1601,22 @@
       <c r="K4" s="15">
         <v>0.89</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="34" t="s">
         <v>92</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
       <c r="B5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>55</v>
       </c>
       <c r="D5" t="s">
@@ -1473,22 +1643,22 @@
       <c r="K5" s="15">
         <v>0.9</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="L5" s="34" t="s">
         <v>46</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="N5" s="39" t="s">
+      <c r="N5" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
       <c r="B6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="35" t="s">
         <v>55</v>
       </c>
       <c r="D6" t="s">
@@ -1515,22 +1685,22 @@
       <c r="K6" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="34" t="s">
         <v>94</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="N6" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="39"/>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
       <c r="B7" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>54</v>
       </c>
       <c r="D7" t="s">
@@ -1557,22 +1727,22 @@
       <c r="K7" s="15">
         <v>0.95</v>
       </c>
-      <c r="L7" s="35" t="s">
+      <c r="L7" s="34" t="s">
         <v>91</v>
       </c>
       <c r="M7" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="N7" s="39" t="s">
+      <c r="N7" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="39"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
       <c r="B8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>54</v>
       </c>
       <c r="D8" t="s">
@@ -1599,22 +1769,22 @@
       <c r="K8" s="15">
         <v>0.46</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="32" t="s">
         <v>132</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="39"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
       <c r="B9" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>53</v>
       </c>
       <c r="D9" t="s">
@@ -1641,22 +1811,22 @@
       <c r="K9" t="s">
         <v>56</v>
       </c>
-      <c r="L9" s="35" t="s">
+      <c r="L9" s="34" t="s">
         <v>96</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
       <c r="B10" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="35" t="s">
         <v>61</v>
       </c>
       <c r="D10" t="s">
@@ -1683,22 +1853,22 @@
       <c r="K10" s="15">
         <v>0.46</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="34" t="s">
         <v>127</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="N10" s="39" t="s">
+      <c r="N10" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="39"/>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
       <c r="B11" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="35" t="s">
         <v>63</v>
       </c>
       <c r="D11" t="s">
@@ -1725,22 +1895,22 @@
       <c r="K11" s="15">
         <v>0.46</v>
       </c>
-      <c r="L11" s="35" t="s">
+      <c r="L11" s="34" t="s">
         <v>128</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="N11" s="39" t="s">
+      <c r="N11" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="39"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
       <c r="B12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="35" t="s">
         <v>60</v>
       </c>
       <c r="D12" t="s">
@@ -1767,22 +1937,22 @@
       <c r="K12" s="15">
         <v>0.91</v>
       </c>
-      <c r="L12" s="35" t="s">
+      <c r="L12" s="34" t="s">
         <v>98</v>
       </c>
       <c r="M12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="N12" s="39" t="s">
+      <c r="N12" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="39"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
       <c r="B13" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="35" t="s">
         <v>81</v>
       </c>
       <c r="D13" t="s">
@@ -1809,22 +1979,22 @@
       <c r="K13" s="15">
         <v>0.91</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="L13" s="32" t="s">
         <v>44</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="N13" s="39" t="s">
+      <c r="N13" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="39"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
       <c r="B14" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="35" t="s">
         <v>79</v>
       </c>
       <c r="D14" t="s">
@@ -1851,22 +2021,22 @@
       <c r="K14" s="15">
         <v>0.91</v>
       </c>
-      <c r="L14" s="33" t="s">
+      <c r="L14" s="32" t="s">
         <v>44</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="N14" s="39" t="s">
+      <c r="N14" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="39"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
       <c r="B15" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="35" t="s">
         <v>79</v>
       </c>
       <c r="D15" t="s">
@@ -1893,22 +2063,22 @@
       <c r="K15" s="15">
         <v>0.91</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="L15" s="32" t="s">
         <v>44</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="N15" s="39" t="s">
+      <c r="N15" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="39"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
       <c r="B16" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="35" t="s">
         <v>79</v>
       </c>
       <c r="D16" t="s">
@@ -1935,22 +2105,22 @@
       <c r="K16" s="15">
         <v>0.91</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="L16" s="32" t="s">
         <v>130</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="N16" s="39" t="s">
+      <c r="N16" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="39"/>
+    <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
       <c r="B17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="35" t="s">
         <v>120</v>
       </c>
       <c r="D17" t="s">
@@ -1977,22 +2147,22 @@
       <c r="K17" s="15">
         <v>0.94</v>
       </c>
-      <c r="L17" s="33" t="s">
+      <c r="L17" s="32" t="s">
         <v>129</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="N17" s="39" t="s">
+      <c r="N17" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="39"/>
+    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
       <c r="B18" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="36" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -2019,31 +2189,31 @@
       <c r="K18" s="20">
         <v>0.96</v>
       </c>
-      <c r="L18" s="34" t="s">
+      <c r="L18" s="33" t="s">
         <v>116</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="N18" s="39" t="s">
+      <c r="N18" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2059,14 +2229,275 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CF52D-B276-4F82-9BD5-373648110EE9}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{6B8190E1-EFD9-4405-88A3-D3F0B878A904}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B52607-E879-4A77-A1A1-581676134552}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" display="https://www.lko.at/holz+2400++1298002" xr:uid="{B2AF2985-3683-4FF9-B776-809EB5AD6C5E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>